<commit_message>
case5 from zoom review
</commit_message>
<xml_diff>
--- a/Case Study 4/Case4 Results.xlsx
+++ b/Case Study 4/Case4 Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickfontenot/Dropbox/SMU/DS7333 Quantifying World/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickfontenot/Dropbox/SMU/DS7333 Quantifying World/QTW_Github/QTW/Case Study 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2649F2E0-208F-AA4A-BEDB-9B2FF822CC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B70A87B-A35B-014A-86BC-A0F999476FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1500" windowWidth="27560" windowHeight="15100" xr2:uid="{5266E1DA-A53B-2A4D-9BE0-F08A195680B7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23620" windowHeight="15440" xr2:uid="{5266E1DA-A53B-2A4D-9BE0-F08A195680B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet6" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>precision</t>
   </si>
@@ -56,24 +56,9 @@
     <t>weighted avg</t>
   </si>
   <si>
-    <t>Subject tf-idf</t>
-  </si>
-  <si>
-    <t>Not_Spam</t>
-  </si>
-  <si>
     <t>Spam</t>
   </si>
   <si>
-    <t>Body tf-idf</t>
-  </si>
-  <si>
-    <t>Subject + Body tf-idf</t>
-  </si>
-  <si>
-    <t>Subject + Body tf-idf + clustering</t>
-  </si>
-  <si>
     <t>easy_ham</t>
   </si>
   <si>
@@ -99,6 +84,33 @@
   </si>
   <si>
     <t>Folder</t>
+  </si>
+  <si>
+    <t>Not Bankrupt</t>
+  </si>
+  <si>
+    <t>Bankrupt</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Tuned</t>
+  </si>
+  <si>
+    <t>SMOTE Resampling</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>Class Weights for imbalance</t>
+  </si>
+  <si>
+    <t>Scale_pos_weight for imbalance</t>
   </si>
 </sst>
 </file>
@@ -106,9 +118,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,8 +135,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,18 +167,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00D662"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -350,11 +372,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -367,12 +457,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,8 +479,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,12 +521,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,362 +841,718 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6257049C-B17E-3540-ADA1-0561D997AB8A}">
-  <dimension ref="B1:R9"/>
+  <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="Q9" sqref="B2:Q9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="17" width="11.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="15" t="s">
+    <row r="2" spans="2:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+    </row>
+    <row r="3" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="29"/>
+    </row>
+    <row r="4" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q5" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="11">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.98</v>
       </c>
-      <c r="D4" s="3">
+      <c r="F6" s="4"/>
+      <c r="G6" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="I6" s="14">
         <v>0.98</v>
       </c>
-      <c r="E4" s="3">
+      <c r="J6" s="4"/>
+      <c r="K6" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="L6" s="14">
         <v>0.98</v>
       </c>
-      <c r="F4" s="4">
-        <v>696</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0.99</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>696</v>
-      </c>
-      <c r="K4" s="29">
-        <v>0.99</v>
-      </c>
-      <c r="L4" s="30">
-        <v>1</v>
-      </c>
-      <c r="M4" s="30">
-        <v>1</v>
-      </c>
-      <c r="N4" s="31">
-        <v>696</v>
-      </c>
-      <c r="O4" s="11">
-        <v>0.99</v>
-      </c>
-      <c r="P4" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.93</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="F5" s="4">
-        <v>240</v>
-      </c>
-      <c r="G5" s="13">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="M6" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="11">
         <v>0.97</v>
       </c>
-      <c r="I5" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="J5" s="4">
-        <v>240</v>
-      </c>
-      <c r="K5" s="32">
-        <v>1</v>
-      </c>
-      <c r="L5" s="33">
+      <c r="P6" s="14">
         <v>0.98</v>
       </c>
-      <c r="M5" s="33">
-        <v>0.99</v>
-      </c>
-      <c r="N5" s="31">
-        <v>240</v>
-      </c>
-      <c r="O5" s="13">
-        <v>1</v>
-      </c>
-      <c r="P5" s="3">
+      <c r="Q6" s="18">
         <v>0.98</v>
       </c>
-      <c r="Q5" s="4">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" ht="11" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="13">
+        <v>0.54</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="11" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="12">
+      <c r="C9" s="5"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="12">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="26">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="19">
+        <v>0.95399999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="13">
+        <v>0.86</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="13">
+        <v>0.76</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="P11" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="33"/>
+    </row>
+    <row r="15" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
+    </row>
+    <row r="16" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="29"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="11">
         <v>0.97</v>
       </c>
-      <c r="F7" s="4">
-        <v>936</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="12">
-        <v>0.99350000000000005</v>
-      </c>
-      <c r="J7" s="4">
-        <v>936</v>
-      </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="39">
-        <v>0.99465000000000003</v>
-      </c>
-      <c r="N7" s="31">
-        <v>936</v>
-      </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="22">
-        <v>0.99465000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="40">
+        <v>0.98</v>
+      </c>
+      <c r="H18" s="41">
+        <v>1</v>
+      </c>
+      <c r="I18" s="41">
+        <v>0.99</v>
+      </c>
+      <c r="J18" s="42"/>
+      <c r="K18" s="5">
+        <v>0.98</v>
+      </c>
+      <c r="L18" s="14">
+        <v>0.97</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0.97</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="11">
+        <v>0.98</v>
+      </c>
+      <c r="P18" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="Q18" s="18">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="43">
+        <v>0.92</v>
+      </c>
+      <c r="H19" s="41">
+        <v>0.6</v>
+      </c>
+      <c r="I19" s="44">
+        <v>0.72</v>
+      </c>
+      <c r="J19" s="42"/>
+      <c r="K19" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="50">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J21" s="42"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="26">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="19">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C22" s="2">
         <v>0.96</v>
       </c>
-      <c r="D8" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="F8" s="4">
-        <v>936</v>
-      </c>
-      <c r="G8" s="13">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="J8" s="4">
-        <v>936</v>
-      </c>
-      <c r="K8" s="32">
-        <v>1</v>
-      </c>
-      <c r="L8" s="33">
-        <v>0.99</v>
-      </c>
-      <c r="M8" s="33">
-        <v>0.99</v>
-      </c>
-      <c r="N8" s="31">
-        <v>936</v>
-      </c>
-      <c r="O8" s="13">
-        <v>1</v>
-      </c>
-      <c r="P8" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="D22" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="43">
+        <v>0.95</v>
+      </c>
+      <c r="H22" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="I22" s="44">
+        <v>0.86</v>
+      </c>
+      <c r="J22" s="42"/>
+      <c r="K22" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="N22" s="4"/>
+      <c r="O22" s="13">
+        <v>0.92</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C23" s="7">
         <v>0.97</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D23" s="8">
         <v>0.97</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E23" s="8">
         <v>0.97</v>
       </c>
-      <c r="F9" s="9">
-        <v>936</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0.99</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0.99</v>
-      </c>
-      <c r="J9" s="9">
-        <v>936</v>
-      </c>
-      <c r="K9" s="36">
-        <v>0.99</v>
-      </c>
-      <c r="L9" s="37">
-        <v>0.99</v>
-      </c>
-      <c r="M9" s="37">
-        <v>0.99</v>
-      </c>
-      <c r="N9" s="38">
-        <v>936</v>
-      </c>
-      <c r="O9" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="P9" s="8">
-        <v>0.99</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>0.99</v>
+      <c r="F23" s="9"/>
+      <c r="G23" s="47">
+        <v>0.98</v>
+      </c>
+      <c r="H23" s="48">
+        <v>0.98</v>
+      </c>
+      <c r="I23" s="48">
+        <v>0.98</v>
+      </c>
+      <c r="J23" s="49"/>
+      <c r="K23" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="N23" s="9"/>
+      <c r="O23" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:Q2"/>
+  <mergeCells count="14">
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="C14:Q14"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1102,77 +1568,77 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="40"/>
-    <col min="4" max="4" width="11.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="40"/>
+    <col min="1" max="3" width="10.83203125" style="20"/>
+    <col min="4" max="4" width="11.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D2" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>19</v>
+      <c r="D2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D3" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="41">
+      <c r="D3" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="21">
         <v>5052</v>
       </c>
-      <c r="F3" s="41" t="s">
-        <v>20</v>
+      <c r="F3" s="21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D4" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="41">
+      <c r="D4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="21">
         <v>1401</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>20</v>
+      <c r="F4" s="21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="21">
+        <v>501</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="41">
-        <v>501</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D6" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="41">
+      <c r="D6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="21">
         <v>1001</v>
       </c>
-      <c r="F6" s="41" t="s">
-        <v>9</v>
+      <c r="F6" s="21" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D7" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="41">
+      <c r="D7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="21">
         <v>1398</v>
       </c>
-      <c r="F7" s="41" t="s">
-        <v>9</v>
+      <c r="F7" s="21" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>